<commit_message>
Fixed Ferrite Bead Resistance
</commit_message>
<xml_diff>
--- a/PCB_Design/PCB/Component List.xlsx
+++ b/PCB_Design/PCB/Component List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\course info\Research\Porto\DDS_on Eurocard_rack\PCB\carrier_board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tujun\Documents\GitHub\DDS-Controller\PCB_Design\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D2688E-9FF2-41D9-8D35-C7323986DE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA8882-A0A9-416F-A119-36B93E4BEE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Part</t>
   </si>
@@ -78,173 +78,210 @@
     <t>523-132134</t>
   </si>
   <si>
+    <t>998-MIC5209-5.0YU</t>
+  </si>
+  <si>
+    <t>621-AS431BNTR-G1</t>
+  </si>
+  <si>
+    <t>581-AEF1010221M035R</t>
+  </si>
+  <si>
+    <t>81-GRM188Z71C225KE3D</t>
+  </si>
+  <si>
+    <t>791-0603B471J500CT</t>
+  </si>
+  <si>
+    <t>80-C0603C104J4RAC</t>
+  </si>
+  <si>
+    <t>81-BLM18KG102SN1D</t>
+  </si>
+  <si>
+    <t>603-RT0603BRD071KL</t>
+  </si>
+  <si>
+    <t>10 kOhm Resistor (3V low-tolerence)</t>
+  </si>
+  <si>
+    <t>603-RT0603BRD1310KL</t>
+  </si>
+  <si>
+    <t>603-RT0603BRD07560KL</t>
+  </si>
+  <si>
+    <t>603-RT0603BRD07220KL</t>
+  </si>
+  <si>
+    <t>603-RT0603BRD07100KL</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE13100RL</t>
+  </si>
+  <si>
+    <t>OPA340UA/2K5</t>
+  </si>
+  <si>
+    <t>187-CL31B106KAHNFNE</t>
+  </si>
+  <si>
+    <t>Cont/brd</t>
+  </si>
+  <si>
+    <t>667-ERA-3AEB123V</t>
+  </si>
+  <si>
+    <t>594-MCT06030C3000FP5</t>
+  </si>
+  <si>
+    <t>603-RT0603BRD0720KL</t>
+  </si>
+  <si>
+    <t>20 kOhm Resistor (10V)</t>
+  </si>
+  <si>
+    <t>1 kOhm Resistor (2.5V)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1kOhm Ferrite </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teensy 4.1 or RPI Pico</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 Ohm Resistor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300 Ohm Resistor (3.6V)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20 Ohm Resistor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT0603FRE0720RLCT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIP SWITCH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD Pinheader 2x3 1.27mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TDD01H0SB1R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S9012E-03-ND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(Part Number)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carlos' DDS Board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	96 Position Din Connector Header Right Angle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>86094647113755ELF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NHD-C0216CZ-FSW-FBW-3V3 (with extra mounting board and 0805 150 Ohm resistor, 2 x 1 uF 0805b capacitors)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 Position Rectangular Receptacle Connector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REC16K25-201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rotational Encoder with press</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMA Cable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>135111-01-06.00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB Micro ccable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>206  Adafruit Industries cable ensemble</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3258 Adafruit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need this time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heat Sinks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71600-008LF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 for R, 5 for C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Through hole 6-pin headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Through hole 2x4-pin headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD 2x4-pin headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G800LQ302018HR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Through hole 24-pin headers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>801-87-024-10-001101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Through hole 24-pin sockets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>757-TLP2767TPE</t>
-  </si>
-  <si>
-    <t>998-MIC5209-5.0YU</t>
-  </si>
-  <si>
-    <t>621-AS431BNTR-G1</t>
-  </si>
-  <si>
-    <t>581-AEF1010221M035R</t>
-  </si>
-  <si>
-    <t>81-GRM188Z71C225KE3D</t>
-  </si>
-  <si>
-    <t>791-0603B471J500CT</t>
-  </si>
-  <si>
-    <t>80-C0603C104J4RAC</t>
-  </si>
-  <si>
-    <t>81-BLM18KG102SN1D</t>
-  </si>
-  <si>
-    <t>603-RT0603BRD071KL</t>
-  </si>
-  <si>
-    <t>10 kOhm Resistor (3V low-tolerence)</t>
-  </si>
-  <si>
-    <t>603-RT0603BRD1310KL</t>
-  </si>
-  <si>
-    <t>603-RT0603BRD07560KL</t>
-  </si>
-  <si>
-    <t>603-RT0603BRD07220KL</t>
-  </si>
-  <si>
-    <t>603-RT0603BRD07100KL</t>
-  </si>
-  <si>
-    <t>603-RT0603FRE13100RL</t>
-  </si>
-  <si>
-    <t>OPA340UA/2K5</t>
-  </si>
-  <si>
-    <t>187-CL31B106KAHNFNE</t>
-  </si>
-  <si>
-    <t>Cont/brd</t>
-  </si>
-  <si>
-    <t>667-ERA-3AEB123V</t>
-  </si>
-  <si>
-    <t>594-MCT06030C3000FP5</t>
-  </si>
-  <si>
-    <t>603-RT0603BRD0720KL</t>
-  </si>
-  <si>
-    <t>20 kOhm Resistor (10V)</t>
-  </si>
-  <si>
-    <t>1 kOhm Resistor (2.5V)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1kOhm Ferrite </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Teensy 4.1 or RPI Pico</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 Ohm Resistor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>300 Ohm Resistor (3.6V)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20 Ohm Resistor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT0603FRE0720RLCT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DIP SWITCH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMD Pinheader 2x3 1.27mm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TDD01H0SB1R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S9012E-03-ND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(Part Number)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Carlos' DDS Board</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Through hole pinheaders/sockets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">	96 Position Din Connector Header Right Angle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>86094647113755ELF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NHD-C0216CZ-FSW-FBW-3V3 (with extra mounting board and 0805 150 Ohm resistor, 2 x 1 uF 0805b capacitors)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6 Position Rectangular Receptacle Connector</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71600-006LF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REC16K25-201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rotational Encoder with press</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMA Cable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>135111-01-06.00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB Micro ccable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>206  Adafruit Industries cable ensemble</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3258 Adafruit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -576,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -587,24 +624,27 @@
     <col min="1" max="1" width="62.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="1"/>
+    <col min="4" max="4" width="28.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="107" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -614,8 +654,11 @@
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -623,10 +666,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -634,10 +680,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -645,10 +694,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -656,10 +708,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -667,12 +722,15 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -680,52 +738,67 @@
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -733,10 +806,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -744,10 +820,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -755,10 +834,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -766,43 +848,55 @@
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -810,10 +904,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -821,10 +918,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -832,10 +932,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -843,114 +946,214 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="1">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="D31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
       <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>61302411121</v>
+      </c>
+      <c r="D36" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>61300821121</v>
+      </c>
+      <c r="D38" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>61030821121</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>